<commit_message>
KARMEN-1 DPE adapted changes in variable names from DD and changed some harmonisation rules accordingly
</commit_message>
<xml_diff>
--- a/analyst/Franzi/rmonize/data_proc_elem/DPE_KARMEN_FRANZI.xlsx
+++ b/analyst/Franzi/rmonize/data_proc_elem/DPE_KARMEN_FRANZI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\Franzi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Franzi\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A9A886-6955-41F6-B525-888A645856C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{A6F9CDCF-C49D-4F92-8C8D-824480319257}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="323">
   <si>
     <t>index</t>
   </si>
@@ -784,111 +784,9 @@
     <t>impossible</t>
   </si>
   <si>
-    <t>Gem02_1</t>
-  </si>
-  <si>
-    <t>Gem02_2</t>
-  </si>
-  <si>
-    <t>Gem02_Hu</t>
-  </si>
-  <si>
-    <t>Obst_sum</t>
-  </si>
-  <si>
-    <t>Nusa_sum</t>
-  </si>
-  <si>
-    <t>Milc_sum</t>
-  </si>
-  <si>
-    <t>Milc07_1</t>
-  </si>
-  <si>
-    <t>Milc07_2</t>
-  </si>
-  <si>
-    <t>Sues13_6</t>
-  </si>
-  <si>
-    <t>Brot_sum</t>
-  </si>
-  <si>
-    <t>Brot01_1</t>
-  </si>
-  <si>
-    <t>Flei_sum</t>
-  </si>
-  <si>
-    <t>Flei_Wurst</t>
-  </si>
-  <si>
-    <t>Fish_sum</t>
-  </si>
-  <si>
-    <t>Fett_sum</t>
-  </si>
-  <si>
-    <t>Sues_sum</t>
-  </si>
-  <si>
-    <t>Sues13_1</t>
-  </si>
-  <si>
-    <t>Sues13_2</t>
-  </si>
-  <si>
-    <t>Getr15_1</t>
-  </si>
-  <si>
-    <t>Getr15_14</t>
-  </si>
-  <si>
-    <t>Getr15_16</t>
-  </si>
-  <si>
-    <t>Getr15_12</t>
-  </si>
-  <si>
-    <t>Getr15_13</t>
-  </si>
-  <si>
-    <t>Getr15_11</t>
-  </si>
-  <si>
-    <t>Getr15_2</t>
-  </si>
-  <si>
-    <t>Getr15_22</t>
-  </si>
-  <si>
-    <t>Getr15_21</t>
-  </si>
-  <si>
-    <t>Getr15_23</t>
-  </si>
-  <si>
-    <t>Getr15_24</t>
-  </si>
-  <si>
-    <t>Sose_sum</t>
-  </si>
-  <si>
-    <t>Supp_sum</t>
-  </si>
-  <si>
-    <t>Sonst_sum</t>
-  </si>
-  <si>
-    <t>Suessstoffe</t>
-  </si>
-  <si>
     <t>direct_mapping</t>
   </si>
   <si>
-    <t>in this case, this combined group only consists of potatoes and no other tubers</t>
-  </si>
-  <si>
     <t>partial</t>
   </si>
   <si>
@@ -907,48 +805,18 @@
     <t>operation</t>
   </si>
   <si>
-    <t>tentative</t>
-  </si>
-  <si>
-    <t>0.5 * Sues13_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">partial </t>
-  </si>
-  <si>
-    <t>Getr15_12 + Getr15_13</t>
-  </si>
-  <si>
     <t>compatible</t>
   </si>
   <si>
-    <t>0.5 * Getr15_12</t>
-  </si>
-  <si>
     <t>__BLANK__</t>
   </si>
   <si>
     <t>paste</t>
   </si>
   <si>
-    <t>2 (24HDR)</t>
-  </si>
-  <si>
     <t>Kart_sum_NCI</t>
   </si>
   <si>
-    <t>tba</t>
-  </si>
-  <si>
-    <t>Would it be possible to calculate % of milk intake from the group Milc07_1? </t>
-  </si>
-  <si>
-    <t>Zu geringe Anzahl an Konsumenten für Berechnung via NCI-Methode (Recall1: n=2; Recall2: n=3) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Would it be possible to calculate % of cheese intake from the group Milc07_2? </t>
-  </si>
-  <si>
     <t>Pasta_rice_NCI</t>
   </si>
   <si>
@@ -994,26 +862,140 @@
     <t>Soyproducts_NCI</t>
   </si>
   <si>
-    <t xml:space="preserve">Would it be possible to calculate % of cheese curd, quark and cottage intake from the group Milc07_2? </t>
-  </si>
-  <si>
-    <t>Do you know the proportion of coffee drinkers? Does 50% make sense?</t>
-  </si>
-  <si>
-    <t>Do you know the proportion of tea drinkers? Does 50% make sense?</t>
-  </si>
-  <si>
     <t>Crackers_NCI</t>
   </si>
   <si>
-    <t>Getr15_12;Getr15_13</t>
+    <t>Gem02_1_NCI</t>
+  </si>
+  <si>
+    <t>Gem02_2_NCI</t>
+  </si>
+  <si>
+    <t>Gem02_Hu_NCI</t>
+  </si>
+  <si>
+    <t>Obst_sum_NCI</t>
+  </si>
+  <si>
+    <t>Nusa_sum_NCI</t>
+  </si>
+  <si>
+    <t>Milc_sum_NCI</t>
+  </si>
+  <si>
+    <t>milk_NCI</t>
+  </si>
+  <si>
+    <t>milkbased_bev_NCI</t>
+  </si>
+  <si>
+    <t>quark_curd_NCI</t>
+  </si>
+  <si>
+    <t>cheeses_NCI</t>
+  </si>
+  <si>
+    <t>Sues13_6_NCI</t>
+  </si>
+  <si>
+    <t>Brot_sum_NCI</t>
+  </si>
+  <si>
+    <t>Brot01_1_NCI</t>
+  </si>
+  <si>
+    <t>Flei_sum_NCI</t>
+  </si>
+  <si>
+    <t>Flei_Wurst_NCI</t>
+  </si>
+  <si>
+    <t>Fish_sum_NCI</t>
+  </si>
+  <si>
+    <t>Fett_sum_NCI</t>
+  </si>
+  <si>
+    <t>Sues_sum_NCI</t>
+  </si>
+  <si>
+    <t>chocolate_sweets_NCI</t>
+  </si>
+  <si>
+    <t>nonchoc_sweets_NCI</t>
+  </si>
+  <si>
+    <t>Sues13_2_NCI</t>
+  </si>
+  <si>
+    <t>Getr15_1_NCI</t>
+  </si>
+  <si>
+    <t>Getr15_14_NCI</t>
+  </si>
+  <si>
+    <t>Getr15_16_NCI</t>
+  </si>
+  <si>
+    <t>Getr15_11_NCI</t>
+  </si>
+  <si>
+    <t>Kaffee_NCI</t>
+  </si>
+  <si>
+    <t>blackgreentea_NCI</t>
+  </si>
+  <si>
+    <t>Getr15_13_NCI</t>
+  </si>
+  <si>
+    <t>Kaffee_NCI;blackgreentea_NCI;Getr15_13_NCI</t>
+  </si>
+  <si>
+    <t>Kaffee_NCI+blackgreentea_NCI+Getr15_13_NCI</t>
+  </si>
+  <si>
+    <t>Getr15_2_NCI</t>
+  </si>
+  <si>
+    <t>Getr15_22_NCI</t>
+  </si>
+  <si>
+    <t>Getr15_21_NCI</t>
+  </si>
+  <si>
+    <t>Getr15_23_MW</t>
+  </si>
+  <si>
+    <t>calculated as mean of 2 24h-recalls</t>
+  </si>
+  <si>
+    <t>Getr15_24_MW</t>
+  </si>
+  <si>
+    <t>Sose_sum_NCI</t>
+  </si>
+  <si>
+    <t>Supp_sum_NCI</t>
+  </si>
+  <si>
+    <t>Sonst_sum_NCI</t>
+  </si>
+  <si>
+    <t>Suessstoffe_MW</t>
+  </si>
+  <si>
+    <t>2 (24HDR) NCI method</t>
+  </si>
+  <si>
+    <t>does not contain other tubers than potatoes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1063,30 +1045,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1101,7 +1075,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1120,7 +1094,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1128,29 +1101,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1166,7 +1128,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1488,11 +1450,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I104" sqref="I104"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="65.85546875" customWidth="1"/>
@@ -1551,23 +1513,23 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>304</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>287</v>
+      <c r="F2" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>254</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>289</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>290</v>
+        <v>322</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1580,21 +1542,21 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>304</v>
+      <c r="F3" s="14" t="s">
+        <v>264</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="I3" s="17"/>
+        <v>254</v>
+      </c>
+      <c r="I3" s="14"/>
       <c r="J3" s="6" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1621,7 +1583,7 @@
         <v>253</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1634,21 +1596,21 @@
       <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="18" t="s">
-        <v>254</v>
+      <c r="F5" t="s">
+        <v>281</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="I5" s="17"/>
+        <v>254</v>
+      </c>
+      <c r="I5" s="14"/>
       <c r="J5" s="6" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1675,7 +1637,7 @@
         <v>253</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1702,7 +1664,7 @@
         <v>253</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1729,7 +1691,7 @@
         <v>253</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1756,7 +1718,7 @@
         <v>253</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1769,21 +1731,21 @@
       <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="18" t="s">
-        <v>255</v>
+      <c r="F10" t="s">
+        <v>282</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="I10" s="17"/>
+        <v>254</v>
+      </c>
+      <c r="I10" s="14"/>
       <c r="J10" s="6" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1796,21 +1758,21 @@
       <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>293</v>
+      <c r="F11" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1823,21 +1785,21 @@
       <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>293</v>
+      <c r="F12" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1850,21 +1812,21 @@
       <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>293</v>
+      <c r="F13" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1877,21 +1839,21 @@
       <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>293</v>
+      <c r="F14" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1904,21 +1866,21 @@
       <c r="D15" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>287</v>
+      <c r="F15" t="s">
+        <v>283</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I15" s="3"/>
-      <c r="J15" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>292</v>
+      <c r="J15" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1931,21 +1893,21 @@
       <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K16" s="13" t="s">
-        <v>293</v>
+      <c r="F16" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -1958,21 +1920,21 @@
       <c r="D17" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>287</v>
+      <c r="F17" t="s">
+        <v>284</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I17" s="3"/>
-      <c r="J17" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K17" s="13" t="s">
-        <v>292</v>
+      <c r="J17" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1985,21 +1947,21 @@
       <c r="D18" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K18" s="13" t="s">
-        <v>293</v>
+      <c r="F18" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -2012,21 +1974,21 @@
       <c r="D19" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>287</v>
+      <c r="F19" t="s">
+        <v>285</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I19" s="3"/>
-      <c r="J19" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>292</v>
+      <c r="J19" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -2039,21 +2001,21 @@
       <c r="D20" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K20" s="13" t="s">
-        <v>293</v>
+      <c r="F20" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
@@ -2066,21 +2028,21 @@
       <c r="D21" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K21" s="13" t="s">
-        <v>293</v>
+      <c r="F21" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -2093,21 +2055,21 @@
       <c r="D22" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>287</v>
+      <c r="F22" t="s">
+        <v>286</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I22" s="3"/>
-      <c r="J22" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K22" s="13" t="s">
-        <v>292</v>
+      <c r="J22" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
@@ -2120,23 +2082,21 @@
       <c r="D23" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="H23" s="21" t="s">
-        <v>305</v>
-      </c>
-      <c r="I23" s="21" t="s">
-        <v>306</v>
-      </c>
-      <c r="J23" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K23" s="13" t="s">
-        <v>292</v>
+      <c r="F23" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
@@ -2149,23 +2109,21 @@
       <c r="D24" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="J24" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K24" s="13" t="s">
-        <v>293</v>
+      <c r="F24" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
@@ -2178,21 +2136,21 @@
       <c r="D25" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>287</v>
+      <c r="F25" t="s">
+        <v>268</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="I25" s="3"/>
-      <c r="J25" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K25" s="13" t="s">
-        <v>292</v>
+      <c r="J25" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
@@ -2205,23 +2163,21 @@
       <c r="D26" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="H26" s="21" t="s">
-        <v>305</v>
-      </c>
-      <c r="I26" s="21" t="s">
-        <v>324</v>
-      </c>
-      <c r="J26" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K26" s="13" t="s">
-        <v>292</v>
+      <c r="F26" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -2234,23 +2190,21 @@
       <c r="D27" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="H27" s="21" t="s">
-        <v>305</v>
-      </c>
-      <c r="I27" s="21" t="s">
-        <v>308</v>
-      </c>
-      <c r="J27" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K27" s="13" t="s">
-        <v>292</v>
+      <c r="F27" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K27" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -2263,21 +2217,21 @@
       <c r="D28" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>287</v>
+      <c r="F28" t="s">
+        <v>291</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I28" s="3"/>
-      <c r="J28" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K28" s="13" t="s">
-        <v>292</v>
+      <c r="J28" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
@@ -2290,21 +2244,21 @@
       <c r="D29" t="s">
         <v>13</v>
       </c>
-      <c r="F29" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K29" s="13" t="s">
-        <v>293</v>
+      <c r="F29" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
@@ -2317,21 +2271,21 @@
       <c r="D30" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K30" s="13" t="s">
-        <v>293</v>
+      <c r="F30" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -2344,21 +2298,21 @@
       <c r="D31" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K31" s="13" t="s">
-        <v>293</v>
+      <c r="F31" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K31" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
@@ -2371,21 +2325,21 @@
       <c r="D32" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K32" s="13" t="s">
-        <v>293</v>
+      <c r="F32" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
@@ -2398,21 +2352,21 @@
       <c r="D33" t="s">
         <v>13</v>
       </c>
-      <c r="F33" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H33" s="13" t="s">
-        <v>287</v>
+      <c r="F33" t="s">
+        <v>292</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I33" s="3"/>
-      <c r="J33" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K33" s="13" t="s">
-        <v>292</v>
+      <c r="J33" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
@@ -2426,20 +2380,20 @@
         <v>13</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>313</v>
+        <v>269</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>287</v>
+        <v>254</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
@@ -2453,20 +2407,20 @@
         <v>13</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>309</v>
+        <v>265</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="H35" s="13" t="s">
-        <v>287</v>
+        <v>254</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I35" s="3"/>
       <c r="J35" s="3" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
@@ -2479,21 +2433,21 @@
       <c r="D36" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="G36" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H36" s="13" t="s">
-        <v>287</v>
+      <c r="F36" t="s">
+        <v>293</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I36" s="3"/>
-      <c r="J36" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K36" s="13" t="s">
-        <v>292</v>
+      <c r="J36" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
@@ -2507,20 +2461,20 @@
         <v>13</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="G37" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H37" s="13" t="s">
-        <v>287</v>
+        <v>270</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I37" s="3"/>
-      <c r="J37" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K37" s="13" t="s">
-        <v>292</v>
+      <c r="J37" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
@@ -2534,20 +2488,20 @@
         <v>13</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H38" s="13" t="s">
-        <v>287</v>
+        <v>271</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I38" s="3"/>
-      <c r="J38" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K38" s="13" t="s">
-        <v>292</v>
+      <c r="J38" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
@@ -2561,20 +2515,20 @@
         <v>13</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="G39" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H39" s="13" t="s">
-        <v>287</v>
+        <v>266</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I39" s="3"/>
-      <c r="J39" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K39" s="13" t="s">
-        <v>292</v>
+      <c r="J39" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K39" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
@@ -2588,20 +2542,20 @@
         <v>13</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="G40" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H40" s="13" t="s">
-        <v>287</v>
+        <v>280</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I40" s="3"/>
-      <c r="J40" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K40" s="13" t="s">
-        <v>292</v>
+      <c r="J40" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K40" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
@@ -2615,20 +2569,20 @@
         <v>13</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="G41" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H41" s="13" t="s">
-        <v>287</v>
+        <v>272</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I41" s="3"/>
-      <c r="J41" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K41" s="13" t="s">
-        <v>292</v>
+      <c r="J41" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K41" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
@@ -2641,21 +2595,21 @@
       <c r="D42" t="s">
         <v>13</v>
       </c>
-      <c r="F42" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="G42" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H42" s="13" t="s">
-        <v>287</v>
+      <c r="F42" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I42" s="3"/>
-      <c r="J42" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K42" s="13" t="s">
-        <v>292</v>
+      <c r="J42" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K42" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
@@ -2682,7 +2636,7 @@
         <v>253</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
@@ -2709,7 +2663,7 @@
         <v>253</v>
       </c>
       <c r="K44" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
@@ -2736,7 +2690,7 @@
         <v>253</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
@@ -2763,7 +2717,7 @@
         <v>253</v>
       </c>
       <c r="K46" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
@@ -2790,7 +2744,7 @@
         <v>253</v>
       </c>
       <c r="K47" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
@@ -2817,7 +2771,7 @@
         <v>253</v>
       </c>
       <c r="K48" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
@@ -2844,7 +2798,7 @@
         <v>253</v>
       </c>
       <c r="K49" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
@@ -2871,7 +2825,7 @@
         <v>253</v>
       </c>
       <c r="K50" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
@@ -2898,7 +2852,7 @@
         <v>253</v>
       </c>
       <c r="K51" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
@@ -2925,7 +2879,7 @@
         <v>253</v>
       </c>
       <c r="K52" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
@@ -2952,7 +2906,7 @@
         <v>253</v>
       </c>
       <c r="K53" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
@@ -2979,7 +2933,7 @@
         <v>253</v>
       </c>
       <c r="K54" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
@@ -3006,7 +2960,7 @@
         <v>253</v>
       </c>
       <c r="K55" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
@@ -3033,7 +2987,7 @@
         <v>253</v>
       </c>
       <c r="K56" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
@@ -3060,7 +3014,7 @@
         <v>253</v>
       </c>
       <c r="K57" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
@@ -3073,21 +3027,21 @@
       <c r="D58" t="s">
         <v>13</v>
       </c>
-      <c r="F58" s="10" t="s">
-        <v>266</v>
+      <c r="F58" s="7" t="s">
+        <v>295</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="H58" s="13" t="s">
-        <v>287</v>
+        <v>254</v>
+      </c>
+      <c r="H58" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I58" s="8"/>
       <c r="J58" s="9" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="K58" s="9" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
@@ -3114,7 +3068,7 @@
         <v>253</v>
       </c>
       <c r="K59" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
@@ -3127,21 +3081,21 @@
       <c r="D60" t="s">
         <v>13</v>
       </c>
-      <c r="F60" s="10" t="s">
-        <v>267</v>
+      <c r="F60" s="7" t="s">
+        <v>296</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="H60" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="I60" s="8"/>
       <c r="J60" s="9" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="K60" s="9" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.25">
@@ -3168,7 +3122,7 @@
         <v>253</v>
       </c>
       <c r="K61" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
@@ -3195,7 +3149,7 @@
         <v>253</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
@@ -3222,7 +3176,7 @@
         <v>253</v>
       </c>
       <c r="K63" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
@@ -3235,21 +3189,21 @@
       <c r="D64" t="s">
         <v>13</v>
       </c>
-      <c r="F64" s="12" t="s">
-        <v>311</v>
+      <c r="F64" s="11" t="s">
+        <v>267</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="H64" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="I64" s="8"/>
       <c r="J64" s="9" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="K64" s="9" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.25">
@@ -3276,7 +3230,7 @@
         <v>253</v>
       </c>
       <c r="K65" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.25">
@@ -3289,21 +3243,21 @@
       <c r="D66" t="s">
         <v>13</v>
       </c>
-      <c r="F66" s="10" t="s">
-        <v>268</v>
+      <c r="F66" s="7" t="s">
+        <v>297</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="H66" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="I66" s="8"/>
       <c r="J66" s="9" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="K66" s="9" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.25">
@@ -3317,20 +3271,20 @@
         <v>13</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="G67" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H67" s="13" t="s">
-        <v>287</v>
+        <v>273</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I67" s="3"/>
-      <c r="J67" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K67" s="13" t="s">
-        <v>292</v>
+      <c r="J67" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K67" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.25">
@@ -3344,20 +3298,20 @@
         <v>13</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="G68" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H68" s="13" t="s">
-        <v>287</v>
+        <v>274</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H68" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I68" s="3"/>
-      <c r="J68" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K68" s="13" t="s">
-        <v>292</v>
+      <c r="J68" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K68" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.25">
@@ -3371,20 +3325,20 @@
         <v>13</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="G69" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H69" s="13" t="s">
-        <v>287</v>
+        <v>275</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H69" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I69" s="3"/>
-      <c r="J69" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K69" s="13" t="s">
-        <v>292</v>
+      <c r="J69" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K69" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.25">
@@ -3397,21 +3351,21 @@
       <c r="D70" t="s">
         <v>13</v>
       </c>
-      <c r="F70" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G70" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H70" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I70" s="13"/>
-      <c r="J70" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K70" s="13" t="s">
-        <v>293</v>
+      <c r="F70" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H70" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I70" s="12"/>
+      <c r="J70" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K70" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.25">
@@ -3424,21 +3378,21 @@
       <c r="D71" t="s">
         <v>13</v>
       </c>
-      <c r="F71" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G71" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H71" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I71" s="13"/>
-      <c r="J71" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K71" s="13" t="s">
-        <v>293</v>
+      <c r="F71" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G71" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H71" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I71" s="12"/>
+      <c r="J71" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K71" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.25">
@@ -3452,20 +3406,20 @@
         <v>13</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="G72" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H72" s="13" t="s">
-        <v>287</v>
+        <v>276</v>
+      </c>
+      <c r="G72" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H72" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I72" s="3"/>
-      <c r="J72" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K72" s="13" t="s">
-        <v>292</v>
+      <c r="J72" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K72" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.25">
@@ -3478,21 +3432,21 @@
       <c r="D73" t="s">
         <v>13</v>
       </c>
-      <c r="F73" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="G73" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H73" s="13" t="s">
-        <v>287</v>
+      <c r="F73" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="G73" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H73" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I73" s="3"/>
-      <c r="J73" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K73" s="13" t="s">
-        <v>292</v>
+      <c r="J73" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K73" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.25">
@@ -3519,7 +3473,7 @@
         <v>253</v>
       </c>
       <c r="K74" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.25">
@@ -3532,21 +3486,21 @@
       <c r="D75" t="s">
         <v>13</v>
       </c>
-      <c r="F75" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="G75" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="H75" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="I75" s="8"/>
-      <c r="J75" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="K75" s="9" t="s">
-        <v>295</v>
+      <c r="F75" t="s">
+        <v>299</v>
+      </c>
+      <c r="G75" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H75" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="I75" s="3"/>
+      <c r="J75" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K75" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
@@ -3559,21 +3513,21 @@
       <c r="D76" t="s">
         <v>13</v>
       </c>
-      <c r="F76" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="G76" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="H76" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="I76" s="8"/>
-      <c r="J76" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="K76" s="9" t="s">
-        <v>295</v>
+      <c r="F76" t="s">
+        <v>300</v>
+      </c>
+      <c r="G76" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H76" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="I76" s="3"/>
+      <c r="J76" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K76" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.25">
@@ -3600,7 +3554,7 @@
         <v>253</v>
       </c>
       <c r="K77" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.25">
@@ -3613,21 +3567,21 @@
       <c r="D78" t="s">
         <v>13</v>
       </c>
-      <c r="F78" s="10" t="s">
-        <v>271</v>
+      <c r="F78" s="15" t="s">
+        <v>301</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="H78" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="I78" s="9"/>
       <c r="J78" s="9" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="K78" s="9" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.25">
@@ -3654,7 +3608,7 @@
         <v>253</v>
       </c>
       <c r="K79" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.25">
@@ -3681,7 +3635,7 @@
         <v>253</v>
       </c>
       <c r="K80" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.25">
@@ -3708,7 +3662,7 @@
         <v>253</v>
       </c>
       <c r="K81" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.25">
@@ -3721,21 +3675,21 @@
       <c r="D82" t="s">
         <v>13</v>
       </c>
-      <c r="F82" s="11" t="s">
-        <v>321</v>
+      <c r="F82" s="10" t="s">
+        <v>277</v>
       </c>
       <c r="G82" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="H82" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="I82" s="9"/>
       <c r="J82" s="9" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="K82" s="9" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.25">
@@ -3762,7 +3716,7 @@
         <v>253</v>
       </c>
       <c r="K83" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.25">
@@ -3789,7 +3743,7 @@
         <v>253</v>
       </c>
       <c r="K84" s="9" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.25">
@@ -3802,21 +3756,21 @@
       <c r="D85" t="s">
         <v>13</v>
       </c>
-      <c r="F85" s="10" t="s">
-        <v>272</v>
+      <c r="F85" s="15" t="s">
+        <v>302</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="H85" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="I85" s="8"/>
       <c r="J85" s="9" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="K85" s="9" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.25">
@@ -3829,21 +3783,21 @@
       <c r="D86" t="s">
         <v>13</v>
       </c>
-      <c r="F86" s="10" t="s">
-        <v>273</v>
+      <c r="F86" s="15" t="s">
+        <v>303</v>
       </c>
       <c r="G86" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="H86" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="I86" s="8"/>
       <c r="J86" s="9" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="K86" s="9" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.25">
@@ -3856,21 +3810,21 @@
       <c r="D87" t="s">
         <v>13</v>
       </c>
-      <c r="F87" s="10" t="s">
-        <v>274</v>
+      <c r="F87" s="15" t="s">
+        <v>304</v>
       </c>
       <c r="G87" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="H87" s="9" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="I87" s="8"/>
       <c r="J87" s="9" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="K87" s="9" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.25">
@@ -3883,21 +3837,21 @@
       <c r="D88" t="s">
         <v>13</v>
       </c>
-      <c r="F88" s="19" t="s">
-        <v>328</v>
-      </c>
-      <c r="G88" s="13" t="s">
-        <v>294</v>
+      <c r="F88" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="G88" s="12" t="s">
+        <v>260</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="I88" s="3"/>
-      <c r="J88" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K88" s="13" t="s">
-        <v>299</v>
+      <c r="J88" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K88" s="12" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.25">
@@ -3910,23 +3864,21 @@
       <c r="D89" t="s">
         <v>13</v>
       </c>
-      <c r="F89" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="G89" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="H89" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="I89" s="21" t="s">
-        <v>325</v>
-      </c>
-      <c r="J89" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="K89" s="13" t="s">
-        <v>295</v>
+      <c r="F89" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="H89" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="I89" s="8"/>
+      <c r="J89" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="K89" s="9" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.25">
@@ -3939,23 +3891,21 @@
       <c r="D90" t="s">
         <v>13</v>
       </c>
-      <c r="F90" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="G90" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="H90" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="I90" s="21" t="s">
-        <v>326</v>
-      </c>
-      <c r="J90" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="K90" s="13" t="s">
-        <v>295</v>
+      <c r="F90" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="H90" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="I90" s="8"/>
+      <c r="J90" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="K90" s="9" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.25">
@@ -3968,21 +3918,21 @@
       <c r="D91" t="s">
         <v>13</v>
       </c>
-      <c r="F91" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="G91" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H91" s="13" t="s">
-        <v>287</v>
+      <c r="F91" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="G91" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H91" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I91" s="3"/>
-      <c r="J91" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K91" s="13" t="s">
-        <v>292</v>
+      <c r="J91" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K91" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.25">
@@ -3995,21 +3945,21 @@
       <c r="D92" t="s">
         <v>13</v>
       </c>
-      <c r="F92" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G92" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H92" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I92" s="13"/>
-      <c r="J92" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K92" s="13" t="s">
-        <v>293</v>
+      <c r="F92" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G92" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H92" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I92" s="12"/>
+      <c r="J92" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K92" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.25">
@@ -4023,20 +3973,20 @@
         <v>13</v>
       </c>
       <c r="F93" s="15" t="s">
-        <v>277</v>
-      </c>
-      <c r="G93" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H93" s="13" t="s">
-        <v>287</v>
+        <v>305</v>
+      </c>
+      <c r="G93" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H93" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I93" s="3"/>
-      <c r="J93" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K93" s="13" t="s">
-        <v>292</v>
+      <c r="J93" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K93" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.25">
@@ -4049,21 +3999,21 @@
       <c r="D94" t="s">
         <v>13</v>
       </c>
-      <c r="F94" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="G94" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H94" s="13" t="s">
-        <v>287</v>
+      <c r="F94" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="G94" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H94" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I94" s="3"/>
-      <c r="J94" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K94" s="13" t="s">
-        <v>292</v>
+      <c r="J94" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K94" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.25">
@@ -4076,21 +4026,21 @@
       <c r="D95" t="s">
         <v>13</v>
       </c>
-      <c r="F95" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="G95" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H95" s="13" t="s">
-        <v>287</v>
+      <c r="F95" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="G95" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H95" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I95" s="3"/>
-      <c r="J95" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K95" s="13" t="s">
-        <v>292</v>
+      <c r="J95" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K95" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.25">
@@ -4103,21 +4053,21 @@
       <c r="D96" t="s">
         <v>13</v>
       </c>
-      <c r="F96" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G96" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H96" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I96" s="13"/>
-      <c r="J96" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K96" s="13" t="s">
-        <v>293</v>
+      <c r="F96" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G96" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H96" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I96" s="12"/>
+      <c r="J96" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K96" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="97" spans="2:11" x14ac:dyDescent="0.25">
@@ -4130,21 +4080,21 @@
       <c r="D97" t="s">
         <v>13</v>
       </c>
-      <c r="F97" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="G97" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H97" s="13" t="s">
-        <v>287</v>
+      <c r="F97" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="G97" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H97" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I97" s="3"/>
-      <c r="J97" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K97" s="13" t="s">
-        <v>292</v>
+      <c r="J97" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K97" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="98" spans="2:11" x14ac:dyDescent="0.25">
@@ -4157,21 +4107,23 @@
       <c r="D98" t="s">
         <v>13</v>
       </c>
-      <c r="F98" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="G98" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H98" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="I98" s="3"/>
-      <c r="J98" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K98" s="13" t="s">
-        <v>292</v>
+      <c r="F98" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="G98" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H98" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="J98" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="K98" s="12" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="99" spans="2:11" x14ac:dyDescent="0.25">
@@ -4184,21 +4136,21 @@
       <c r="D99" t="s">
         <v>13</v>
       </c>
-      <c r="F99" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G99" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H99" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I99" s="13"/>
-      <c r="J99" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K99" s="13" t="s">
-        <v>293</v>
+      <c r="F99" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G99" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H99" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I99" s="12"/>
+      <c r="J99" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K99" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="100" spans="2:11" x14ac:dyDescent="0.25">
@@ -4211,21 +4163,21 @@
       <c r="D100" t="s">
         <v>13</v>
       </c>
-      <c r="F100" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G100" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H100" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I100" s="13"/>
-      <c r="J100" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K100" s="13" t="s">
-        <v>293</v>
+      <c r="F100" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G100" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H100" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I100" s="12"/>
+      <c r="J100" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K100" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="101" spans="2:11" x14ac:dyDescent="0.25">
@@ -4238,21 +4190,23 @@
       <c r="D101" t="s">
         <v>13</v>
       </c>
-      <c r="F101" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="G101" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H101" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="I101" s="3"/>
-      <c r="J101" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K101" s="13" t="s">
-        <v>292</v>
+      <c r="F101" s="17" t="s">
+        <v>316</v>
+      </c>
+      <c r="G101" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H101" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="I101" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="J101" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="K101" s="12" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="102" spans="2:11" x14ac:dyDescent="0.25">
@@ -4265,21 +4219,21 @@
       <c r="D102" t="s">
         <v>13</v>
       </c>
-      <c r="F102" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="G102" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H102" s="13" t="s">
-        <v>287</v>
+      <c r="F102" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="G102" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H102" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I102" s="3"/>
-      <c r="J102" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K102" s="13" t="s">
-        <v>292</v>
+      <c r="J102" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K102" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="103" spans="2:11" x14ac:dyDescent="0.25">
@@ -4292,21 +4246,21 @@
       <c r="D103" t="s">
         <v>13</v>
       </c>
-      <c r="F103" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G103" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H103" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I103" s="13"/>
-      <c r="J103" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K103" s="13" t="s">
-        <v>293</v>
+      <c r="F103" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G103" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H103" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I103" s="12"/>
+      <c r="J103" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K103" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="104" spans="2:11" x14ac:dyDescent="0.25">
@@ -4319,21 +4273,21 @@
       <c r="D104" t="s">
         <v>13</v>
       </c>
-      <c r="F104" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G104" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H104" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I104" s="13"/>
-      <c r="J104" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K104" s="13" t="s">
-        <v>293</v>
+      <c r="F104" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G104" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H104" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I104" s="12"/>
+      <c r="J104" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K104" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="105" spans="2:11" x14ac:dyDescent="0.25">
@@ -4346,21 +4300,21 @@
       <c r="D105" t="s">
         <v>13</v>
       </c>
-      <c r="F105" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G105" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H105" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I105" s="13"/>
-      <c r="J105" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K105" s="13" t="s">
-        <v>293</v>
+      <c r="F105" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G105" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H105" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I105" s="12"/>
+      <c r="J105" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K105" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="106" spans="2:11" x14ac:dyDescent="0.25">
@@ -4373,21 +4327,21 @@
       <c r="D106" t="s">
         <v>13</v>
       </c>
-      <c r="F106" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G106" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H106" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I106" s="13"/>
-      <c r="J106" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K106" s="13" t="s">
-        <v>293</v>
+      <c r="F106" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G106" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H106" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I106" s="12"/>
+      <c r="J106" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K106" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="107" spans="2:11" x14ac:dyDescent="0.25">
@@ -4400,21 +4354,21 @@
       <c r="D107" t="s">
         <v>13</v>
       </c>
-      <c r="F107" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G107" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H107" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I107" s="13"/>
-      <c r="J107" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K107" s="13" t="s">
-        <v>293</v>
+      <c r="F107" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G107" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H107" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I107" s="12"/>
+      <c r="J107" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K107" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="108" spans="2:11" x14ac:dyDescent="0.25">
@@ -4427,21 +4381,21 @@
       <c r="D108" t="s">
         <v>13</v>
       </c>
-      <c r="F108" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G108" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H108" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I108" s="13"/>
-      <c r="J108" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K108" s="13" t="s">
-        <v>293</v>
+      <c r="F108" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G108" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H108" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I108" s="12"/>
+      <c r="J108" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K108" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="109" spans="2:11" x14ac:dyDescent="0.25">
@@ -4454,21 +4408,21 @@
       <c r="D109" t="s">
         <v>13</v>
       </c>
-      <c r="F109" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G109" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H109" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I109" s="13"/>
-      <c r="J109" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K109" s="13" t="s">
-        <v>293</v>
+      <c r="F109" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G109" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H109" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I109" s="12"/>
+      <c r="J109" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K109" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="110" spans="2:11" x14ac:dyDescent="0.25">
@@ -4481,21 +4435,21 @@
       <c r="D110" t="s">
         <v>13</v>
       </c>
-      <c r="F110" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G110" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="H110" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="I110" s="13"/>
-      <c r="J110" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K110" s="13" t="s">
-        <v>293</v>
+      <c r="F110" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G110" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H110" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="I110" s="12"/>
+      <c r="J110" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K110" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="111" spans="2:11" x14ac:dyDescent="0.25">
@@ -4508,21 +4462,21 @@
       <c r="D111" t="s">
         <v>13</v>
       </c>
-      <c r="F111" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="G111" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H111" s="13" t="s">
-        <v>287</v>
+      <c r="F111" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="G111" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H111" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I111" s="3"/>
-      <c r="J111" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K111" s="13" t="s">
-        <v>292</v>
+      <c r="J111" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K111" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="112" spans="2:11" x14ac:dyDescent="0.25">
@@ -4535,21 +4489,21 @@
       <c r="D112" t="s">
         <v>13</v>
       </c>
-      <c r="F112" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G112" s="13" t="s">
+      <c r="F112" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G112" s="12" t="s">
         <v>253</v>
       </c>
       <c r="H112" s="3" t="s">
         <v>253</v>
       </c>
       <c r="I112" s="3"/>
-      <c r="J112" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K112" s="13" t="s">
-        <v>293</v>
+      <c r="J112" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K112" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="113" spans="2:11" x14ac:dyDescent="0.25">
@@ -4562,21 +4516,21 @@
       <c r="D113" t="s">
         <v>13</v>
       </c>
-      <c r="F113" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G113" s="13" t="s">
+      <c r="F113" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G113" s="12" t="s">
         <v>253</v>
       </c>
       <c r="H113" s="3" t="s">
         <v>253</v>
       </c>
       <c r="I113" s="3"/>
-      <c r="J113" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K113" s="13" t="s">
-        <v>293</v>
+      <c r="J113" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K113" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="114" spans="2:11" x14ac:dyDescent="0.25">
@@ -4589,21 +4543,21 @@
       <c r="D114" t="s">
         <v>13</v>
       </c>
-      <c r="F114" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="G114" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H114" s="13" t="s">
-        <v>287</v>
+      <c r="F114" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="G114" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H114" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I114" s="3"/>
-      <c r="J114" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K114" s="13" t="s">
-        <v>292</v>
+      <c r="J114" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K114" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="115" spans="2:11" x14ac:dyDescent="0.25">
@@ -4616,21 +4570,21 @@
       <c r="D115" t="s">
         <v>13</v>
       </c>
-      <c r="F115" s="16" t="s">
-        <v>322</v>
-      </c>
-      <c r="G115" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H115" s="13" t="s">
-        <v>287</v>
+      <c r="F115" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="G115" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H115" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I115" s="3"/>
-      <c r="J115" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K115" s="13" t="s">
-        <v>292</v>
+      <c r="J115" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K115" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="116" spans="2:11" x14ac:dyDescent="0.25">
@@ -4643,21 +4597,21 @@
       <c r="D116" t="s">
         <v>13</v>
       </c>
-      <c r="F116" s="16" t="s">
-        <v>323</v>
-      </c>
-      <c r="G116" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H116" s="13" t="s">
-        <v>287</v>
+      <c r="F116" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="G116" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H116" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="I116" s="3"/>
-      <c r="J116" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K116" s="13" t="s">
-        <v>292</v>
+      <c r="J116" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="K116" s="12" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="117" spans="2:11" x14ac:dyDescent="0.25">
@@ -4670,21 +4624,21 @@
       <c r="D117" t="s">
         <v>13</v>
       </c>
-      <c r="F117" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G117" s="13" t="s">
+      <c r="F117" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G117" s="12" t="s">
         <v>253</v>
       </c>
       <c r="H117" s="3" t="s">
         <v>253</v>
       </c>
       <c r="I117" s="3"/>
-      <c r="J117" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K117" s="13" t="s">
-        <v>293</v>
+      <c r="J117" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K117" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="118" spans="2:11" x14ac:dyDescent="0.25">
@@ -4697,21 +4651,23 @@
       <c r="D118" t="s">
         <v>13</v>
       </c>
-      <c r="F118" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="G118" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="H118" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="I118" s="3"/>
-      <c r="J118" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="K118" s="13" t="s">
-        <v>292</v>
+      <c r="F118" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="G118" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="H118" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="J118" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="K118" s="12" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="119" spans="2:11" x14ac:dyDescent="0.25">
@@ -4724,21 +4680,21 @@
       <c r="D119" t="s">
         <v>13</v>
       </c>
-      <c r="F119" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G119" s="13" t="s">
+      <c r="F119" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G119" s="12" t="s">
         <v>253</v>
       </c>
       <c r="H119" s="3" t="s">
         <v>253</v>
       </c>
       <c r="I119" s="3"/>
-      <c r="J119" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K119" s="13" t="s">
-        <v>293</v>
+      <c r="J119" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K119" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="120" spans="2:11" x14ac:dyDescent="0.25">
@@ -4751,21 +4707,21 @@
       <c r="D120" t="s">
         <v>13</v>
       </c>
-      <c r="F120" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="G120" s="13" t="s">
+      <c r="F120" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G120" s="12" t="s">
         <v>253</v>
       </c>
       <c r="H120" s="3" t="s">
         <v>253</v>
       </c>
       <c r="I120" s="3"/>
-      <c r="J120" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K120" s="13" t="s">
-        <v>293</v>
+      <c r="J120" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="K120" s="12" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="121" spans="2:11" x14ac:dyDescent="0.25">
@@ -4779,22 +4735,22 @@
         <v>252</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>301</v>
+        <v>262</v>
       </c>
       <c r="G121" s="5" t="s">
-        <v>302</v>
+        <v>263</v>
       </c>
       <c r="H121">
         <v>2</v>
       </c>
       <c r="I121" s="7" t="s">
-        <v>303</v>
+        <v>321</v>
       </c>
       <c r="J121" s="6" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="K121" s="6" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>